<commit_message>
Reto de liga 19 enero
</commit_message>
<xml_diff>
--- a/torneos/TOTALTORNEOS.xlsx
+++ b/torneos/TOTALTORNEOS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\beyblade apps\TorneoTablas\torneos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD90793-2543-4596-A89E-CD99FB42AE23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069BA1EF-9573-4B6E-95BC-1927410BAD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2904" yWindow="2904" windowWidth="23472" windowHeight="14376" xr2:uid="{CB882399-940D-4B8B-9F67-A952E17FF4BE}"/>
+    <workbookView xWindow="3456" yWindow="2904" windowWidth="23544" windowHeight="14376" xr2:uid="{CB882399-940D-4B8B-9F67-A952E17FF4BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="130">
   <si>
     <t>POSICION</t>
   </si>
@@ -141,9 +141,6 @@
     <t>QRO000055</t>
   </si>
   <si>
-    <t>MAU</t>
-  </si>
-  <si>
     <t>QRO000056</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
     <t>QRO000015</t>
   </si>
   <si>
-    <t>OSO</t>
-  </si>
-  <si>
     <t>QRO000036</t>
   </si>
   <si>
@@ -394,6 +388,45 @@
   </si>
   <si>
     <t>QRO000052</t>
+  </si>
+  <si>
+    <t>OZZO</t>
+  </si>
+  <si>
+    <t>MAURELIO</t>
+  </si>
+  <si>
+    <t>QRO000057</t>
+  </si>
+  <si>
+    <t>FRANCHESCA</t>
+  </si>
+  <si>
+    <t>QRO000058</t>
+  </si>
+  <si>
+    <t>L0FTY65</t>
+  </si>
+  <si>
+    <t>QRO000061</t>
+  </si>
+  <si>
+    <t>HECTOR0819</t>
+  </si>
+  <si>
+    <t>QRO000059</t>
+  </si>
+  <si>
+    <t>ELIAN0516</t>
+  </si>
+  <si>
+    <t>QRO000060</t>
+  </si>
+  <si>
+    <t>KITTY</t>
+  </si>
+  <si>
+    <t>QRO000062</t>
   </si>
 </sst>
 </file>
@@ -520,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -539,6 +572,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -854,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05D896B-943C-43C0-94BD-76348AD6D6F0}">
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -889,28 +940,28 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="10">
+        <v>3</v>
+      </c>
+      <c r="E2" s="10">
+        <v>192</v>
+      </c>
+      <c r="F2" s="10">
         <v>2</v>
       </c>
-      <c r="E2" s="6">
-        <v>90</v>
-      </c>
-      <c r="F2" s="6">
-        <v>1</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6">
+      <c r="G2" s="10">
+        <v>0</v>
+      </c>
+      <c r="H2" s="10">
         <v>1</v>
       </c>
     </row>
@@ -925,10 +976,10 @@
         <v>11</v>
       </c>
       <c r="D3" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" s="6">
-        <v>79</v>
+        <v>140</v>
       </c>
       <c r="F3" s="6">
         <v>1</v>
@@ -945,22 +996,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D4" s="6">
+        <v>3</v>
+      </c>
+      <c r="E4" s="6">
+        <v>138</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
         <v>2</v>
-      </c>
-      <c r="E4" s="6">
-        <v>78</v>
-      </c>
-      <c r="F4" s="6">
-        <v>1</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0</v>
       </c>
       <c r="H4" s="6">
         <v>0</v>
@@ -971,16 +1022,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D5" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="6">
-        <v>62</v>
+        <v>120</v>
       </c>
       <c r="F5" s="6">
         <v>0</v>
@@ -997,22 +1048,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D6" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="6">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="F6" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="6">
         <v>0</v>
@@ -1023,16 +1074,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D7" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="6">
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="F7" s="6">
         <v>0</v>
@@ -1049,25 +1100,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D8" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" s="6">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="F8" s="6">
         <v>0</v>
       </c>
       <c r="G8" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1075,22 +1126,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D9" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9" s="6">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="F9" s="6">
         <v>0</v>
       </c>
       <c r="G9" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" s="6">
         <v>0</v>
@@ -1101,16 +1152,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D10" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E10" s="6">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="F10" s="6">
         <v>0</v>
@@ -1127,16 +1178,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>26</v>
+        <v>117</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="D11" s="6">
         <v>2</v>
       </c>
       <c r="E11" s="6">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="F11" s="6">
         <v>0</v>
@@ -1145,7 +1196,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1153,16 +1204,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>28</v>
+        <v>118</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D12" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="6">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="F12" s="6">
         <v>0</v>
@@ -1174,21 +1225,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>31</v>
+        <v>119</v>
       </c>
       <c r="D13" s="6">
         <v>1</v>
       </c>
       <c r="E13" s="6">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="F13" s="6">
         <v>0</v>
@@ -1205,16 +1256,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>32</v>
+        <v>120</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>33</v>
+        <v>121</v>
       </c>
       <c r="D14" s="6">
         <v>1</v>
       </c>
       <c r="E14" s="6">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="F14" s="6">
         <v>0</v>
@@ -1231,16 +1282,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>34</v>
+        <v>122</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>35</v>
+        <v>123</v>
       </c>
       <c r="D15" s="6">
         <v>1</v>
       </c>
       <c r="E15" s="6">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="F15" s="6">
         <v>0</v>
@@ -1252,47 +1303,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D16" s="6">
+        <v>2</v>
+      </c>
+      <c r="E16" s="6">
+        <v>56</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0</v>
+      </c>
+      <c r="H16" s="6">
         <v>1</v>
-      </c>
-      <c r="E16" s="6">
-        <v>23</v>
-      </c>
-      <c r="F16" s="6">
-        <v>0</v>
-      </c>
-      <c r="G16" s="6">
-        <v>0</v>
-      </c>
-      <c r="H16" s="6">
-        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D17" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" s="6">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="F17" s="6">
         <v>0</v>
@@ -1304,21 +1355,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="D18" s="6">
         <v>1</v>
       </c>
       <c r="E18" s="6">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="F18" s="6">
         <v>0</v>
@@ -1335,16 +1386,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>42</v>
+        <v>126</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>43</v>
+        <v>127</v>
       </c>
       <c r="D19" s="6">
         <v>1</v>
       </c>
       <c r="E19" s="6">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="F19" s="6">
         <v>0</v>
@@ -1358,19 +1409,19 @@
     </row>
     <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="D20" s="6">
         <v>1</v>
       </c>
       <c r="E20" s="6">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="F20" s="6">
         <v>0</v>
@@ -1382,21 +1433,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D21" s="6">
         <v>1</v>
       </c>
       <c r="E21" s="6">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="F21" s="6">
         <v>0</v>
@@ -1408,21 +1459,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="D22" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="6">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="F22" s="6">
         <v>0</v>
@@ -1436,19 +1487,19 @@
     </row>
     <row r="23" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="D23" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="6">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="F23" s="6">
         <v>0</v>
@@ -1460,21 +1511,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="D24" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="6">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F24" s="6">
         <v>0</v>
@@ -1488,19 +1539,19 @@
     </row>
     <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D25" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="6">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F25" s="6">
         <v>0</v>
@@ -1514,19 +1565,19 @@
     </row>
     <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D26" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="6">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F26" s="6">
         <v>0</v>
@@ -1538,21 +1589,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D27" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="6">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F27" s="6">
         <v>0</v>
@@ -1564,15 +1615,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="D28" s="6">
         <v>0</v>
@@ -1590,15 +1641,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="D29" s="6">
         <v>0</v>
@@ -1618,13 +1669,13 @@
     </row>
     <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D30" s="6">
         <v>0</v>
@@ -1644,13 +1695,13 @@
     </row>
     <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D31" s="6">
         <v>0</v>
@@ -1670,13 +1721,13 @@
     </row>
     <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D32" s="6">
         <v>0</v>
@@ -1696,13 +1747,13 @@
     </row>
     <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D33" s="6">
         <v>0</v>
@@ -1720,15 +1771,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D34" s="6">
         <v>0</v>
@@ -1748,13 +1799,13 @@
     </row>
     <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D35" s="6">
         <v>0</v>
@@ -1774,13 +1825,13 @@
     </row>
     <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="D36" s="6">
         <v>0</v>
@@ -1798,15 +1849,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="D37" s="6">
         <v>0</v>
@@ -1826,13 +1877,13 @@
     </row>
     <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="D38" s="6">
         <v>0</v>
@@ -1852,13 +1903,13 @@
     </row>
     <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="D39" s="6">
         <v>0</v>
@@ -1878,13 +1929,13 @@
     </row>
     <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="D40" s="6">
         <v>0</v>
@@ -1904,13 +1955,13 @@
     </row>
     <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="D41" s="6">
         <v>0</v>
@@ -1930,13 +1981,13 @@
     </row>
     <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="D42" s="6">
         <v>0</v>
@@ -1954,15 +2005,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D43" s="6">
         <v>0</v>
@@ -1980,15 +2031,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="D44" s="6">
         <v>0</v>
@@ -2008,13 +2059,13 @@
     </row>
     <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D45" s="6">
         <v>0</v>
@@ -2034,13 +2085,13 @@
     </row>
     <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="D46" s="6">
         <v>0</v>
@@ -2060,13 +2111,13 @@
     </row>
     <row r="47" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="D47" s="6">
         <v>0</v>
@@ -2086,13 +2137,13 @@
     </row>
     <row r="48" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D48" s="6">
         <v>0</v>
@@ -2112,13 +2163,13 @@
     </row>
     <row r="49" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="D49" s="6">
         <v>0</v>
@@ -2136,15 +2187,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="D50" s="6">
         <v>0</v>
@@ -2162,15 +2213,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="D51" s="6">
         <v>0</v>
@@ -2190,13 +2241,13 @@
     </row>
     <row r="52" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="D52" s="6">
         <v>0</v>
@@ -2216,13 +2267,13 @@
     </row>
     <row r="53" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="D53" s="6">
         <v>0</v>
@@ -2240,15 +2291,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="D54" s="6">
         <v>0</v>
@@ -2268,81 +2319,277 @@
     </row>
     <row r="55" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B55" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D55" s="6">
+        <v>0</v>
+      </c>
+      <c r="E55" s="6">
+        <v>0</v>
+      </c>
+      <c r="F55" s="6">
+        <v>0</v>
+      </c>
+      <c r="G55" s="6">
+        <v>0</v>
+      </c>
+      <c r="H55" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="3">
+        <v>27</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D56" s="6">
+        <v>0</v>
+      </c>
+      <c r="E56" s="6">
+        <v>0</v>
+      </c>
+      <c r="F56" s="6">
+        <v>0</v>
+      </c>
+      <c r="G56" s="6">
+        <v>0</v>
+      </c>
+      <c r="H56" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="3">
+        <v>27</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D57" s="6">
+        <v>0</v>
+      </c>
+      <c r="E57" s="6">
+        <v>0</v>
+      </c>
+      <c r="F57" s="6">
+        <v>0</v>
+      </c>
+      <c r="G57" s="6">
+        <v>0</v>
+      </c>
+      <c r="H57" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="3">
+        <v>27</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D58" s="6">
+        <v>0</v>
+      </c>
+      <c r="E58" s="6">
+        <v>0</v>
+      </c>
+      <c r="F58" s="6">
+        <v>0</v>
+      </c>
+      <c r="G58" s="6">
+        <v>0</v>
+      </c>
+      <c r="H58" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="3">
+        <v>27</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D59" s="6">
+        <v>0</v>
+      </c>
+      <c r="E59" s="6">
+        <v>0</v>
+      </c>
+      <c r="F59" s="6">
+        <v>0</v>
+      </c>
+      <c r="G59" s="6">
+        <v>0</v>
+      </c>
+      <c r="H59" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="3">
+        <v>27</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D60" s="6">
+        <v>0</v>
+      </c>
+      <c r="E60" s="6">
+        <v>0</v>
+      </c>
+      <c r="F60" s="6">
+        <v>0</v>
+      </c>
+      <c r="G60" s="6">
+        <v>0</v>
+      </c>
+      <c r="H60" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="3">
+        <v>27</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D61" s="6">
+        <v>0</v>
+      </c>
+      <c r="E61" s="6">
+        <v>0</v>
+      </c>
+      <c r="F61" s="6">
+        <v>0</v>
+      </c>
+      <c r="G61" s="6">
+        <v>0</v>
+      </c>
+      <c r="H61" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="3">
+        <v>27</v>
+      </c>
+      <c r="B62" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C62" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D55" s="6">
-        <v>0</v>
-      </c>
-      <c r="E55" s="6">
-        <v>0</v>
-      </c>
-      <c r="F55" s="6">
-        <v>0</v>
-      </c>
-      <c r="G55" s="6">
-        <v>0</v>
-      </c>
-      <c r="H55" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="3">
-        <v>21</v>
-      </c>
-      <c r="B56" s="4" t="s">
+      <c r="D62" s="6">
+        <v>0</v>
+      </c>
+      <c r="E62" s="6">
+        <v>0</v>
+      </c>
+      <c r="F62" s="6">
+        <v>0</v>
+      </c>
+      <c r="G62" s="6">
+        <v>0</v>
+      </c>
+      <c r="H62" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="3">
+        <v>27</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C63" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D56" s="6">
-        <v>0</v>
-      </c>
-      <c r="E56" s="6">
-        <v>0</v>
-      </c>
-      <c r="F56" s="6">
-        <v>0</v>
-      </c>
-      <c r="G56" s="6">
-        <v>0</v>
-      </c>
-      <c r="H56" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="3">
-        <v>21</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D57" s="6">
-        <v>0</v>
-      </c>
-      <c r="E57" s="6">
-        <v>0</v>
-      </c>
-      <c r="F57" s="6">
-        <v>0</v>
-      </c>
-      <c r="G57" s="6">
-        <v>0</v>
-      </c>
-      <c r="H57" s="6">
-        <v>0</v>
-      </c>
+      <c r="D63" s="6">
+        <v>0</v>
+      </c>
+      <c r="E63" s="6">
+        <v>0</v>
+      </c>
+      <c r="F63" s="6">
+        <v>0</v>
+      </c>
+      <c r="G63" s="6">
+        <v>0</v>
+      </c>
+      <c r="H63" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="11"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+    </row>
+    <row r="65" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="11"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+    </row>
+    <row r="66" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="11"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+    </row>
+    <row r="67" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="11"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
torneo local 25 enenro fix total
</commit_message>
<xml_diff>
--- a/torneos/TOTALTORNEOS.xlsx
+++ b/torneos/TOTALTORNEOS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\beyblade apps\TorneoTablas\torneos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069BA1EF-9573-4B6E-95BC-1927410BAD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3951A68-B0DC-407E-9668-84ECE0D46B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3456" yWindow="2904" windowWidth="23544" windowHeight="14376" xr2:uid="{CB882399-940D-4B8B-9F67-A952E17FF4BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{CB882399-940D-4B8B-9F67-A952E17FF4BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="134">
   <si>
     <t>POSICION</t>
   </si>
@@ -159,9 +159,6 @@
     <t>QRO000036</t>
   </si>
   <si>
-    <t>GERA</t>
-  </si>
-  <si>
     <t>QRO000045</t>
   </si>
   <si>
@@ -427,6 +424,21 @@
   </si>
   <si>
     <t>QRO000062</t>
+  </si>
+  <si>
+    <t>GARFIELD</t>
+  </si>
+  <si>
+    <t>MEDX</t>
+  </si>
+  <si>
+    <t>QRO000063</t>
+  </si>
+  <si>
+    <t>GHAST1003</t>
+  </si>
+  <si>
+    <t>QRO000064</t>
   </si>
 </sst>
 </file>
@@ -553,7 +565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -571,18 +583,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -907,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05D896B-943C-43C0-94BD-76348AD6D6F0}">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H67"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -940,28 +940,28 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="6">
+        <v>4</v>
+      </c>
+      <c r="E2" s="6">
+        <v>277</v>
+      </c>
+      <c r="F2" s="6">
         <v>3</v>
       </c>
-      <c r="E2" s="10">
-        <v>192</v>
-      </c>
-      <c r="F2" s="10">
-        <v>2</v>
-      </c>
-      <c r="G2" s="10">
-        <v>0</v>
-      </c>
-      <c r="H2" s="10">
+      <c r="G2" s="6">
+        <v>0</v>
+      </c>
+      <c r="H2" s="6">
         <v>1</v>
       </c>
     </row>
@@ -976,16 +976,16 @@
         <v>11</v>
       </c>
       <c r="D3" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3" s="6">
-        <v>140</v>
+        <v>204</v>
       </c>
       <c r="F3" s="6">
         <v>1</v>
       </c>
       <c r="G3" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="6">
         <v>0</v>
@@ -1002,10 +1002,10 @@
         <v>15</v>
       </c>
       <c r="D4" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" s="6">
-        <v>138</v>
+        <v>189</v>
       </c>
       <c r="F4" s="6">
         <v>0</v>
@@ -1022,22 +1022,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D5" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5" s="6">
-        <v>120</v>
+        <v>156</v>
       </c>
       <c r="F5" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="6">
         <v>0</v>
@@ -1045,25 +1045,25 @@
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D6" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" s="6">
-        <v>119</v>
+        <v>156</v>
       </c>
       <c r="F6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="6">
         <v>1</v>
-      </c>
-      <c r="G6" s="6">
-        <v>0</v>
       </c>
       <c r="H6" s="6">
         <v>0</v>
@@ -1074,25 +1074,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D7" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7" s="6">
-        <v>104</v>
+        <v>155</v>
       </c>
       <c r="F7" s="6">
         <v>0</v>
       </c>
       <c r="G7" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1100,25 +1100,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E8" s="6">
-        <v>103</v>
+        <v>153</v>
       </c>
       <c r="F8" s="6">
         <v>0</v>
       </c>
       <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6">
         <v>1</v>
-      </c>
-      <c r="H8" s="6">
-        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1132,10 +1132,10 @@
         <v>25</v>
       </c>
       <c r="D9" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E9" s="6">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="F9" s="6">
         <v>0</v>
@@ -1158,10 +1158,10 @@
         <v>27</v>
       </c>
       <c r="D10" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E10" s="6">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="F10" s="6">
         <v>0</v>
@@ -1178,16 +1178,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>117</v>
+        <v>55</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>39</v>
+        <v>118</v>
       </c>
       <c r="D11" s="6">
         <v>2</v>
       </c>
       <c r="E11" s="6">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="F11" s="6">
         <v>0</v>
@@ -1196,7 +1196,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1204,42 +1204,42 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>118</v>
+        <v>18</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D12" s="6">
+        <v>3</v>
+      </c>
+      <c r="E12" s="6">
+        <v>97</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0</v>
+      </c>
+      <c r="H12" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="6">
         <v>2</v>
       </c>
-      <c r="E12" s="6">
-        <v>64</v>
-      </c>
-      <c r="F12" s="6">
-        <v>0</v>
-      </c>
-      <c r="G12" s="6">
-        <v>0</v>
-      </c>
-      <c r="H12" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
-        <v>11</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D13" s="6">
-        <v>1</v>
-      </c>
       <c r="E13" s="6">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="F13" s="6">
         <v>0</v>
@@ -1251,21 +1251,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D14" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" s="6">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="F14" s="6">
         <v>0</v>
@@ -1282,16 +1282,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>123</v>
+        <v>34</v>
       </c>
       <c r="D15" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E15" s="6">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="F15" s="6">
         <v>0</v>
@@ -1303,21 +1303,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="D16" s="6">
         <v>2</v>
       </c>
       <c r="E16" s="6">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="F16" s="6">
         <v>0</v>
@@ -1331,45 +1331,45 @@
     </row>
     <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="D17" s="6">
+        <v>3</v>
+      </c>
+      <c r="E17" s="6">
+        <v>83</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="6">
         <v>2</v>
       </c>
-      <c r="E17" s="6">
-        <v>56</v>
-      </c>
-      <c r="F17" s="6">
-        <v>0</v>
-      </c>
-      <c r="G17" s="6">
-        <v>0</v>
-      </c>
-      <c r="H17" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3">
-        <v>17</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D18" s="6">
-        <v>1</v>
-      </c>
       <c r="E18" s="6">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="F18" s="6">
         <v>0</v>
@@ -1386,42 +1386,42 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>127</v>
+        <v>39</v>
       </c>
       <c r="D19" s="6">
+        <v>2</v>
+      </c>
+      <c r="E19" s="6">
+        <v>82</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0</v>
+      </c>
+      <c r="G19" s="6">
+        <v>0</v>
+      </c>
+      <c r="H19" s="6">
         <v>1</v>
       </c>
-      <c r="E19" s="6">
-        <v>53</v>
-      </c>
-      <c r="F19" s="6">
-        <v>0</v>
-      </c>
-      <c r="G19" s="6">
-        <v>0</v>
-      </c>
-      <c r="H19" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>128</v>
+        <v>30</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>129</v>
+        <v>31</v>
       </c>
       <c r="D20" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20" s="6">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="F20" s="6">
         <v>0</v>
@@ -1444,10 +1444,10 @@
         <v>29</v>
       </c>
       <c r="D21" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" s="6">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="F21" s="6">
         <v>0</v>
@@ -1464,16 +1464,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>30</v>
+        <v>123</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>31</v>
+        <v>124</v>
       </c>
       <c r="D22" s="6">
         <v>1</v>
       </c>
       <c r="E22" s="6">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="F22" s="6">
         <v>0</v>
@@ -1485,21 +1485,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>32</v>
+        <v>125</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>33</v>
+        <v>126</v>
       </c>
       <c r="D23" s="6">
         <v>1</v>
       </c>
       <c r="E23" s="6">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="F23" s="6">
         <v>0</v>
@@ -1511,21 +1511,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>35</v>
+        <v>130</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>36</v>
+        <v>131</v>
       </c>
       <c r="D24" s="6">
         <v>1</v>
       </c>
       <c r="E24" s="6">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="F24" s="6">
         <v>0</v>
@@ -1537,21 +1537,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D25" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25" s="6">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="F25" s="6">
         <v>0</v>
@@ -1568,16 +1568,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>42</v>
+        <v>132</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
       <c r="D26" s="6">
         <v>1</v>
       </c>
       <c r="E26" s="6">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="F26" s="6">
         <v>0</v>
@@ -1589,21 +1589,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D27" s="6">
         <v>1</v>
       </c>
       <c r="E27" s="6">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F27" s="6">
         <v>0</v>
@@ -1620,16 +1620,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D28" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="6">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F28" s="6">
         <v>0</v>
@@ -1646,16 +1646,16 @@
         <v>27</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D29" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="6">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F29" s="6">
         <v>0</v>
@@ -1669,13 +1669,13 @@
     </row>
     <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D30" s="6">
         <v>0</v>
@@ -1693,15 +1693,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D31" s="6">
         <v>0</v>
@@ -1721,13 +1721,13 @@
     </row>
     <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D32" s="6">
         <v>0</v>
@@ -1747,13 +1747,13 @@
     </row>
     <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D33" s="6">
         <v>0</v>
@@ -1771,15 +1771,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D34" s="6">
         <v>0</v>
@@ -1799,13 +1799,13 @@
     </row>
     <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D35" s="6">
         <v>0</v>
@@ -1823,15 +1823,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D36" s="6">
         <v>0</v>
@@ -1851,13 +1851,13 @@
     </row>
     <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D37" s="6">
         <v>0</v>
@@ -1877,13 +1877,13 @@
     </row>
     <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D38" s="6">
         <v>0</v>
@@ -1903,13 +1903,13 @@
     </row>
     <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D39" s="6">
         <v>0</v>
@@ -1929,13 +1929,13 @@
     </row>
     <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D40" s="6">
         <v>0</v>
@@ -1955,13 +1955,13 @@
     </row>
     <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D41" s="6">
         <v>0</v>
@@ -1981,13 +1981,13 @@
     </row>
     <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D42" s="6">
         <v>0</v>
@@ -2005,15 +2005,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D43" s="6">
         <v>0</v>
@@ -2033,13 +2033,13 @@
     </row>
     <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D44" s="6">
         <v>0</v>
@@ -2057,15 +2057,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D45" s="6">
         <v>0</v>
@@ -2085,13 +2085,13 @@
     </row>
     <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D46" s="6">
         <v>0</v>
@@ -2111,13 +2111,13 @@
     </row>
     <row r="47" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D47" s="6">
         <v>0</v>
@@ -2137,13 +2137,13 @@
     </row>
     <row r="48" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D48" s="6">
         <v>0</v>
@@ -2163,13 +2163,13 @@
     </row>
     <row r="49" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D49" s="6">
         <v>0</v>
@@ -2187,15 +2187,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D50" s="6">
         <v>0</v>
@@ -2215,13 +2215,13 @@
     </row>
     <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D51" s="6">
         <v>0</v>
@@ -2239,15 +2239,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D52" s="6">
         <v>0</v>
@@ -2267,13 +2267,13 @@
     </row>
     <row r="53" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D53" s="6">
         <v>0</v>
@@ -2293,13 +2293,13 @@
     </row>
     <row r="54" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D54" s="6">
         <v>0</v>
@@ -2319,13 +2319,13 @@
     </row>
     <row r="55" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D55" s="6">
         <v>0</v>
@@ -2345,13 +2345,13 @@
     </row>
     <row r="56" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D56" s="6">
         <v>0</v>
@@ -2369,15 +2369,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D57" s="6">
         <v>0</v>
@@ -2397,65 +2397,65 @@
     </row>
     <row r="58" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B58" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D58" s="6">
+        <v>0</v>
+      </c>
+      <c r="E58" s="6">
+        <v>0</v>
+      </c>
+      <c r="F58" s="6">
+        <v>0</v>
+      </c>
+      <c r="G58" s="6">
+        <v>0</v>
+      </c>
+      <c r="H58" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="3">
+        <v>29</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D59" s="6">
+        <v>0</v>
+      </c>
+      <c r="E59" s="6">
+        <v>0</v>
+      </c>
+      <c r="F59" s="6">
+        <v>0</v>
+      </c>
+      <c r="G59" s="6">
+        <v>0</v>
+      </c>
+      <c r="H59" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="3">
+        <v>29</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C60" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D58" s="6">
-        <v>0</v>
-      </c>
-      <c r="E58" s="6">
-        <v>0</v>
-      </c>
-      <c r="F58" s="6">
-        <v>0</v>
-      </c>
-      <c r="G58" s="6">
-        <v>0</v>
-      </c>
-      <c r="H58" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="3">
-        <v>27</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D59" s="6">
-        <v>0</v>
-      </c>
-      <c r="E59" s="6">
-        <v>0</v>
-      </c>
-      <c r="F59" s="6">
-        <v>0</v>
-      </c>
-      <c r="G59" s="6">
-        <v>0</v>
-      </c>
-      <c r="H59" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="3">
-        <v>27</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="D60" s="6">
         <v>0</v>
@@ -2475,13 +2475,13 @@
     </row>
     <row r="61" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D61" s="6">
         <v>0</v>
@@ -2501,13 +2501,13 @@
     </row>
     <row r="62" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D62" s="6">
         <v>0</v>
@@ -2527,54 +2527,86 @@
     </row>
     <row r="63" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B63" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D63" s="6">
+        <v>0</v>
+      </c>
+      <c r="E63" s="6">
+        <v>0</v>
+      </c>
+      <c r="F63" s="6">
+        <v>0</v>
+      </c>
+      <c r="G63" s="6">
+        <v>0</v>
+      </c>
+      <c r="H63" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="3">
+        <v>29</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D64" s="6">
+        <v>0</v>
+      </c>
+      <c r="E64" s="6">
+        <v>0</v>
+      </c>
+      <c r="F64" s="6">
+        <v>0</v>
+      </c>
+      <c r="G64" s="6">
+        <v>0</v>
+      </c>
+      <c r="H64" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="3">
+        <v>29</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C65" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D63" s="6">
-        <v>0</v>
-      </c>
-      <c r="E63" s="6">
-        <v>0</v>
-      </c>
-      <c r="F63" s="6">
-        <v>0</v>
-      </c>
-      <c r="G63" s="6">
-        <v>0</v>
-      </c>
-      <c r="H63" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="11"/>
-      <c r="B64" s="4"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-    </row>
-    <row r="65" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="11"/>
-      <c r="B65" s="4"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
-      <c r="H65" s="4"/>
+      <c r="D65" s="6">
+        <v>0</v>
+      </c>
+      <c r="E65" s="6">
+        <v>0</v>
+      </c>
+      <c r="F65" s="6">
+        <v>0</v>
+      </c>
+      <c r="G65" s="6">
+        <v>0</v>
+      </c>
+      <c r="H65" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="66" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="11"/>
+      <c r="A66" s="7"/>
       <c r="B66" s="4"/>
-      <c r="C66" s="12"/>
+      <c r="C66" s="8"/>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
@@ -2582,9 +2614,9 @@
       <c r="H66" s="4"/>
     </row>
     <row r="67" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="11"/>
+      <c r="A67" s="7"/>
       <c r="B67" s="4"/>
-      <c r="C67" s="12"/>
+      <c r="C67" s="8"/>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>

</xml_diff>